<commit_message>
add total sales record row and multiple databse attachment done.
</commit_message>
<xml_diff>
--- a/Pharmacy/wwwroot/export.xlsx
+++ b/Pharmacy/wwwroot/export.xlsx
@@ -79,9 +79,6 @@
     <x:t>u</x:t>
   </x:si>
   <x:si>
-    <x:t>12</x:t>
-  </x:si>
-  <x:si>
     <x:t>12/28/2023 12:00:00 AM</x:t>
   </x:si>
   <x:si>
@@ -94,7 +91,7 @@
     <x:t>Upper Rack</x:t>
   </x:si>
   <x:si>
-    <x:t>10</x:t>
+    <x:t>4</x:t>
   </x:si>
   <x:si>
     <x:t>Awab</x:t>
@@ -107,6 +104,9 @@
   </x:si>
   <x:si>
     <x:t>lower</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0</x:t>
   </x:si>
   <x:si>
     <x:t>Faizan</x:t>
@@ -556,7 +556,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
         <x:v>15</x:v>
@@ -568,30 +568,30 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="I3" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:9">
       <x:c r="A4" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
         <x:v>23</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>24</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="E4" s="0" t="s">
+      <x:c r="F4" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="F4" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
       <x:c r="G4" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
         <x:v>16</x:v>
@@ -602,19 +602,19 @@
     </x:row>
     <x:row r="5" spans="1:9">
       <x:c r="A5" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>28</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>29</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
         <x:v>30</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>26</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
         <x:v>31</x:v>

</xml_diff>

<commit_message>
Add export and import
</commit_message>
<xml_diff>
--- a/Pharmacy/wwwroot/export.xlsx
+++ b/Pharmacy/wwwroot/export.xlsx
@@ -34,6 +34,9 @@
     <x:t>Manufacturer</x:t>
   </x:si>
   <x:si>
+    <x:t>CategoryName</x:t>
+  </x:si>
+  <x:si>
     <x:t>Supplier</x:t>
   </x:si>
   <x:si>
@@ -43,73 +46,163 @@
     <x:t>ExpDate</x:t>
   </x:si>
   <x:si>
+    <x:t>55</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Panadol</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L3</x:t>
+  </x:si>
+  <x:si>
     <x:t>15</x:t>
   </x:si>
   <x:si>
-    <x:t>Panadol</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Upper rack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rehan</x:t>
+    <x:t>Abode</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cosmetics</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALi</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/10/2023 12:00:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1/14/2024 12:00:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>56</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hair Aid</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1100.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>R4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Medicare</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Khan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/24/2023 12:00:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cofcol</x:t>
+  </x:si>
+  <x:si>
+    <x:t>126.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cafcol</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Surgery</x:t>
   </x:si>
   <x:si>
     <x:t>rehan</x:t>
   </x:si>
   <x:si>
-    <x:t>12/13/2023 12:00:00 AM</x:t>
-  </x:si>
-  <x:si>
     <x:t>12/31/2023 12:00:00 AM</x:t>
   </x:si>
   <x:si>
+    <x:t>58</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fogg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>400.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>k8</x:t>
+  </x:si>
+  <x:si>
     <x:t>16</x:t>
   </x:si>
   <x:si>
-    <x:t>panadol</x:t>
-  </x:si>
-  <x:si>
-    <x:t>u</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12/28/2023 12:00:00 AM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Panadol Cf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Upper Rack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Awab</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Brofen</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lower</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Faizan</x:t>
+    <x:t>fogg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ibtehaj</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/4/2023 12:00:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1/15/2024 12:00:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>l9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ll</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ii</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/11/2023 12:00:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1/1/2024 12:00:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>60</x:t>
+  </x:si>
+  <x:si>
+    <x:t>61</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62</x:t>
+  </x:si>
+  <x:si>
+    <x:t>63</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64</x:t>
+  </x:si>
+  <x:si>
+    <x:t>65</x:t>
+  </x:si>
+  <x:si>
+    <x:t>66</x:t>
+  </x:si>
+  <x:si>
+    <x:t>67</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -173,18 +266,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I5" totalsRowShown="0">
-  <x:autoFilter ref="A1:I5"/>
-  <x:tableColumns count="9">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J14" totalsRowShown="0">
+  <x:autoFilter ref="A1:J14"/>
+  <x:tableColumns count="10">
     <x:tableColumn id="1" name="pk_MedId"/>
     <x:tableColumn id="2" name="Name"/>
     <x:tableColumn id="3" name="UnitPrice"/>
     <x:tableColumn id="4" name="Location"/>
     <x:tableColumn id="5" name="Stock"/>
     <x:tableColumn id="6" name="Manufacturer"/>
-    <x:tableColumn id="7" name="Supplier"/>
-    <x:tableColumn id="8" name="MfgDate"/>
-    <x:tableColumn id="9" name="ExpDate"/>
+    <x:tableColumn id="7" name="CategoryName"/>
+    <x:tableColumn id="8" name="Supplier"/>
+    <x:tableColumn id="9" name="MfgDate"/>
+    <x:tableColumn id="10" name="ExpDate"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -478,13 +572,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:I5"/>
+  <x:dimension ref="A1:J14"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:9">
+    <x:row r="1" spans="1:10">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -512,121 +606,424 @@
       <x:c r="I1" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:9">
+      <x:c r="J1" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:10">
       <x:c r="A2" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:10">
+      <x:c r="A3" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="J3" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:10">
+      <x:c r="A4" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="J4" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:10">
+      <x:c r="A5" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="I5" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="J5" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:10">
+      <x:c r="A6" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="J6" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:10">
+      <x:c r="A7" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="C7" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="E2" s="0" t="s">
+      <x:c r="D7" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="F2" s="0" t="s">
+      <x:c r="E7" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="G2" s="0" t="s">
+      <x:c r="F7" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="H2" s="0" t="s">
+      <x:c r="G7" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="I2" s="0" t="s">
+      <x:c r="H7" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:9">
-      <x:c r="A3" s="0" t="s">
+      <x:c r="I7" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
+      <x:c r="J7" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="C3" s="0" t="s">
+    </x:row>
+    <x:row r="8" spans="1:10">
+      <x:c r="A8" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G8" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H8" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="I8" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="J8" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:10">
+      <x:c r="A9" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H9" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="I9" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="J9" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:10">
+      <x:c r="A10" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="G10" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="H10" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="I10" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="J10" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:10">
+      <x:c r="A11" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
+      <x:c r="C11" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="F3" s="0" t="s">
+      <x:c r="E11" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="G3" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="H3" s="0" t="s">
+      <x:c r="G11" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="I3" s="0" t="s">
+      <x:c r="H11" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="I11" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="J11" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:10">
+      <x:c r="A12" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-    </x:row>
-    <x:row r="4" spans="1:9">
-      <x:c r="A4" s="0" t="s">
+      <x:c r="C12" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s">
+      <x:c r="D12" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
+      <x:c r="E12" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="E4" s="0" t="s">
+      <x:c r="F12" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="F4" s="0" t="s">
+      <x:c r="G12" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H12" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="G4" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="H4" s="0" t="s">
+      <x:c r="I12" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="J12" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:10">
+      <x:c r="A13" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="G13" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="I4" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:9">
-      <x:c r="A5" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="G5" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="I5" s="0" t="s">
-        <x:v>17</x:v>
+      <x:c r="H13" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="I13" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="J13" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:10">
+      <x:c r="A14" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="G14" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="H14" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="I14" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="J14" s="0" t="s">
+        <x:v>54</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>